<commit_message>
Update styling of Members Section
</commit_message>
<xml_diff>
--- a/content/members.xlsx
+++ b/content/members.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="11">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
+    <t xml:space="preserve">link</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gaurav</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lorem De coutij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/ligmitz</t>
   </si>
   <si>
     <t xml:space="preserve">Second</t>
@@ -59,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -93,6 +99,13 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -138,7 +151,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,6 +161,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -168,15 +185,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -186,71 +203,92 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -304,6 +342,14 @@
       <c r="C17" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D4" r:id="rId3" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D5" r:id="rId4" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D6" r:id="rId5" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D7" r:id="rId6" display="https://github.com/ligmitz"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -319,13 +365,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:C17"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
   </cols>
@@ -340,71 +386,92 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -458,6 +525,14 @@
       <c r="C17" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D4" r:id="rId3" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D5" r:id="rId4" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D6" r:id="rId5" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D7" r:id="rId6" display="https://github.com/ligmitz"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -473,15 +548,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:C17"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,71 +569,92 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,6 +708,14 @@
       <c r="C17" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D4" r:id="rId3" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D5" r:id="rId4" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D6" r:id="rId5" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D7" r:id="rId6" display="https://github.com/ligmitz"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -627,13 +731,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="1" sqref="A8:C17 D27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.31"/>
   </cols>
@@ -648,71 +752,92 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -766,6 +891,14 @@
       <c r="C17" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D4" r:id="rId3" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D5" r:id="rId4" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D6" r:id="rId5" display="https://github.com/ligmitz"/>
+    <hyperlink ref="D7" r:id="rId6" display="https://github.com/ligmitz"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Add image fields in sheet
</commit_message>
<xml_diff>
--- a/content/members.xlsx
+++ b/content/members.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="57">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">link</t>
   </si>
   <si>
+    <t xml:space="preserve">img</t>
+  </si>
+  <si>
     <t xml:space="preserve">Binod</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://github.com/ligmitz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./members/balidaan.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Gaurav Pandey</t>
@@ -283,7 +289,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -297,6 +303,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -317,13 +327,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.28"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -338,89 +351,110 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,17 +531,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,201 +558,246 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -762,15 +842,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.65"/>
   </cols>
@@ -788,215 +868,263 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,17 +1166,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,215 +1192,263 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>